<commit_message>
WISEDAG-12 added more snomed concepts
</commit_message>
<xml_diff>
--- a/terms_excel.xlsx
+++ b/terms_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\Master Project\wise-dag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D32B16DB-42A3-4B55-9AFC-1796B3A883CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA817D76-FFB5-446E-B70C-26DAB6498F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1724EB86-F306-47F4-ABEC-FB51705565F8}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="318">
   <si>
     <t>terms</t>
   </si>
@@ -956,6 +956,24 @@
   </si>
   <si>
     <t>na</t>
+  </si>
+  <si>
+    <t>88003-9</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>rate of</t>
+  </si>
+  <si>
+    <t>LOINC</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>in heart</t>
   </si>
 </sst>
 </file>
@@ -1439,8 +1457,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1816,20 +1836,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D181B-FC1A-461E-92A1-3F55E3525786}">
-  <dimension ref="A1:C309"/>
+  <dimension ref="A1:E309"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="42.59765625" customWidth="1"/>
+    <col min="1" max="1" width="67.9296875" customWidth="1"/>
     <col min="2" max="2" width="24.73046875" customWidth="1"/>
     <col min="3" max="3" width="15.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1839,8 +1859,11 @@
       <c r="C1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1848,7 +1871,7 @@
         <v>73211009</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1856,7 +1879,7 @@
         <v>71395006</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1864,7 +1887,7 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1872,7 +1895,7 @@
         <v>59621000</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1880,7 +1903,7 @@
         <v>60621009</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1888,7 +1911,7 @@
         <v>49436004</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1896,7 +1919,7 @@
         <v>365981007</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1904,7 +1927,7 @@
         <v>55822004</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1912,7 +1935,7 @@
         <v>709044004</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1923,7 +1946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1934,7 +1957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1942,7 +1965,7 @@
         <v>246116008</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1950,97 +1973,160 @@
         <v>311</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
+      <c r="B16">
+        <v>273302005</v>
+      </c>
       <c r="C16">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B17" t="s">
+        <v>312</v>
+      </c>
+      <c r="D17" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B18">
+        <v>49436004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B19" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B20" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B21">
+        <v>51308000</v>
+      </c>
+      <c r="D21" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B22">
+        <v>43810009</v>
+      </c>
+      <c r="D22" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B23">
+        <v>28960008</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B24">
+        <v>365981007</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B25">
+        <v>71395006</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B26">
+        <v>73211009</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B27">
+        <v>370992007</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B28">
+        <v>116661000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B29">
+        <v>31996006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B30">
+        <v>204317008</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B31">
+        <v>59621000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
+      </c>
+      <c r="B32">
+        <v>60621009</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -2050,41 +2136,65 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
+      <c r="B33">
+        <v>248153007</v>
+      </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>33</v>
       </c>
+      <c r="B34">
+        <v>73211009</v>
+      </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>34</v>
       </c>
+      <c r="B35">
+        <v>55822004</v>
+      </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>35</v>
       </c>
+      <c r="B36">
+        <v>429775004</v>
+      </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>36</v>
       </c>
+      <c r="B37">
+        <v>226097005</v>
+      </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>37</v>
       </c>
+      <c r="B38">
+        <v>49436004</v>
+      </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>38</v>
       </c>
+      <c r="B39">
+        <v>38716007</v>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>39</v>
       </c>
+      <c r="B40">
+        <v>60621009</v>
+      </c>
       <c r="C40">
         <v>2</v>
       </c>
@@ -2093,36 +2203,60 @@
       <c r="A41" t="s">
         <v>40</v>
       </c>
+      <c r="B41">
+        <v>422504002</v>
+      </c>
+      <c r="C41">
+        <v>1</v>
+      </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>41</v>
       </c>
+      <c r="B42">
+        <v>59621000</v>
+      </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>42</v>
       </c>
+      <c r="B43">
+        <v>51308000</v>
+      </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>43</v>
       </c>
+      <c r="B44">
+        <v>246116008</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>44</v>
       </c>
+      <c r="B45">
+        <v>60621009</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>45</v>
       </c>
+      <c r="B46" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>46</v>
       </c>
+      <c r="B47">
+        <v>422504002</v>
+      </c>
       <c r="C47">
         <v>1</v>
       </c>
@@ -2131,1123 +2265,1650 @@
       <c r="A48" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B48" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B49">
+        <v>31996006</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B50" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B51">
+        <v>90708001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>248153007</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B53">
+        <v>256235009</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B54">
+        <v>370992007</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B55">
+        <v>721961000000100</v>
+      </c>
+      <c r="D55" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B56">
+        <v>422504002</v>
+      </c>
+      <c r="C56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B57">
+        <v>102680009</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B58">
+        <v>56265001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B59">
+        <v>55235003</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B60">
+        <v>226097005</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B61">
+        <v>27550009</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B62">
+        <v>35489007</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B63">
+        <v>405056001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B64">
+        <v>160580001</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B65">
+        <v>257552002</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B66">
+        <v>386806002</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B67">
+        <v>56675007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B68">
+        <v>260678004</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B69">
+        <v>38716007</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B70" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B71">
+        <v>439127006</v>
+      </c>
+      <c r="D71" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B72">
+        <v>48447003</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B73">
+        <v>35489007</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B74">
+        <v>122459003</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B75">
+        <v>40739000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B76">
+        <v>104577001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B77">
+        <v>256235009</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B78">
+        <v>422504002</v>
+      </c>
+      <c r="C78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B79">
+        <v>325141000000103</v>
+      </c>
+      <c r="C79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B80">
+        <v>325141000000103</v>
+      </c>
+      <c r="C80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B81">
+        <v>55822004</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B82">
+        <v>40733004</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B83">
+        <v>7.2649930100011904E+17</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B84">
+        <v>1.68376810001191E+16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B85">
+        <v>422504002</v>
+      </c>
+      <c r="C85">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A86" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B86">
+        <v>91175000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B87">
+        <v>698247007</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B88">
+        <v>248153007</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B89" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A90" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B90">
+        <v>441541008</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A91" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B91">
+        <v>102680009</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A92" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B92">
+        <v>248153007</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A93" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B93">
+        <v>13644009</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A94" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B94">
+        <v>59621000</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A95" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B95">
+        <v>49436004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A96" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B96">
+        <v>22298006</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B97">
+        <v>422504002</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B98">
+        <v>38716007</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B99">
+        <v>260678004</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B100">
+        <v>422504002</v>
+      </c>
+      <c r="C100">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B101">
+        <v>73211009</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B102">
+        <v>459056003</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B103">
+        <v>160580001</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B104">
+        <v>73595000</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B105">
+        <v>315053001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B106">
+        <v>116661000</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B107">
+        <v>308116003</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B108">
+        <v>233604007</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B109">
+        <v>429723008</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B110">
+        <v>40492006</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B111">
+        <v>38013005</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B112">
+        <v>248152002</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A113" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B113">
+        <v>68566005</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A114" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B114" s="1">
+        <v>386725007</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A115" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B115" s="1">
+        <v>2776000</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A116" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B116">
+        <v>309966001</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A117" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B117">
+        <v>14766002</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A118" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B118">
+        <v>248153007</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A119" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B119">
+        <v>55822004</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A120" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B120">
+        <v>22298006</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A121" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B121">
+        <v>246273001</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A122" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B122">
+        <v>103228002</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A123" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B123">
+        <v>21134002</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A124" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B124">
+        <v>165232002</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A125" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B125">
+        <v>44695005</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A126" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B126">
+        <v>128053003</v>
+      </c>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A127" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B127">
+        <v>59282003</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A128" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B128">
+        <v>161898004</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A129" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B129">
+        <v>125605004</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A130" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B130">
+        <v>256235009</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A131" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B131">
+        <v>365458002</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A132" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B132">
+        <v>365550006</v>
+      </c>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A133" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B133">
+        <v>422650009</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A134" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B134">
+        <v>266257000</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A135" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B135">
+        <v>256235009</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A136" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B136">
+        <v>1255163004</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A137" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B137">
+        <v>13644009</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A138" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B138">
+        <v>713081000</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A139" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B139">
+        <v>266894000</v>
+      </c>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A140" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B140">
+        <v>838275008</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A141" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B141">
+        <v>204317008</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A142" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B142">
+        <v>5935008</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A143" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B143">
+        <v>698456001</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A144" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B144">
+        <v>361071000000102</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B145">
+        <v>315053001</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B146">
+        <v>450741005</v>
+      </c>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B147">
+        <v>724787004</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B148">
+        <v>60621009</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B149">
+        <v>73430006</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B150">
+        <v>248152002</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B151">
+        <v>4473006</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>151</v>
       </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B152">
+        <v>48194001</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B153" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B154">
+        <v>237602007</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B155">
+        <v>257552002</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B156" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B157">
+        <v>89743005</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B158">
+        <v>38716007</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B159">
+        <v>105981003</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B160">
+        <v>415582006</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B161" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B162">
+        <v>392031002</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B163">
+        <v>1148582006</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B164">
+        <v>6914000</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="166" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B165">
+        <v>723857007</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="167" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B166">
+        <v>398254007</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="168" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B167">
+        <v>103579009</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="169" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B168">
+        <v>47708004</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="170" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B169">
+        <v>64779008</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="171" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B170">
+        <v>363346000</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="172" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B171">
+        <v>31996006</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="173" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B172">
+        <v>367336001</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="174" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B173">
+        <v>192759008</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="175" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B174">
+        <v>248152002</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="176" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B175">
+        <v>248153007</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B176">
+        <v>77386006</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A177" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B177">
+        <v>56819008</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A178" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B178">
+        <v>76612001</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A179" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B179">
+        <v>276654001</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A180" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B180">
+        <v>1230010003</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A181" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B181">
+        <v>394610002</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A182" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B182">
+        <v>37796009</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A183" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B183">
+        <v>45007003</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A184" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B184">
+        <v>56675007</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A185" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B185">
+        <v>404999000</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A186" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B186">
+        <v>20059004</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A187" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B187">
+        <v>264533003</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A188" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B188">
+        <v>415582006</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A189" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B189">
+        <v>20059004</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A190" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B190" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A191" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B191">
+        <v>710864009</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A192" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B192">
+        <v>1325171000000100</v>
+      </c>
+    </row>
+    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B193">
+        <v>31653004</v>
+      </c>
+    </row>
+    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B194">
+        <v>31996006</v>
+      </c>
+    </row>
+    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B195">
+        <v>69116000</v>
+      </c>
+    </row>
+    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B197">
+        <v>422504002</v>
+      </c>
+    </row>
+    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B200">
+        <v>38716007</v>
+      </c>
+    </row>
+    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="E201" s="2"/>
+    </row>
+    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B202">
+        <v>13644009</v>
+      </c>
+    </row>
+    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B204" s="2"/>
+    </row>
+    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B206">
+        <v>49436004</v>
+      </c>
+    </row>
+    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B207">
+        <v>248153007</v>
+      </c>
+    </row>
+    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B221">
+        <v>315053001</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B222">
+        <v>89362005</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>229</v>
       </c>
     </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B234">
+        <v>428202005</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B235">
+        <v>429775004</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B236">
+        <v>1161000175101</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B237">
+        <v>422504002</v>
+      </c>
+      <c r="C237">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B238">
+        <v>422504002</v>
+      </c>
+      <c r="C238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B241">
+        <v>422504002</v>
+      </c>
+      <c r="C241">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B248">
+        <v>248152002</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B263">
+        <v>256235009</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>271</v>
       </c>
@@ -3281,6 +3942,12 @@
       <c r="A278" t="s">
         <v>277</v>
       </c>
+      <c r="B278">
+        <v>422504002</v>
+      </c>
+      <c r="C278">
+        <v>1</v>
+      </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
@@ -3291,6 +3958,9 @@
       <c r="A280" t="s">
         <v>279</v>
       </c>
+      <c r="B280">
+        <v>450741005</v>
+      </c>
       <c r="C280">
         <v>2</v>
       </c>
@@ -3341,82 +4011,88 @@
         <v>287</v>
       </c>
     </row>
-    <row r="289" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="290" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="291" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="292" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="293" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="294" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="295" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="296" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="297" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="298" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="299" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="300" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="301" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B300">
+        <v>422504002</v>
+      </c>
+      <c r="C300">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="302" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="303" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>302</v>
       </c>
     </row>
-    <row r="304" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
         <v>303</v>
       </c>

</xml_diff>

<commit_message>
WISEDAG-12 added qualifier concepts snomed
</commit_message>
<xml_diff>
--- a/terms_excel.xlsx
+++ b/terms_excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\Master Project\wise-dag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA817D76-FFB5-446E-B70C-26DAB6498F10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CE0B17-0C88-4DB3-898F-9D6F27885C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1724EB86-F306-47F4-ABEC-FB51705565F8}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="329">
   <si>
     <t>terms</t>
   </si>
@@ -961,19 +961,52 @@
     <t>88003-9</t>
   </si>
   <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>rate of</t>
-  </si>
-  <si>
-    <t>LOINC</t>
-  </si>
-  <si>
     <t>low</t>
   </si>
   <si>
     <t>in heart</t>
+  </si>
+  <si>
+    <t>qualifier</t>
+  </si>
+  <si>
+    <t>increased activation</t>
+  </si>
+  <si>
+    <t>qualifier_code</t>
+  </si>
+  <si>
+    <t>time to (delay before)</t>
+  </si>
+  <si>
+    <t>awareness of (known)</t>
+  </si>
+  <si>
+    <t>rate of (speed of delivery)</t>
+  </si>
+  <si>
+    <t>dysfunction</t>
+  </si>
+  <si>
+    <t>psychogenic</t>
+  </si>
+  <si>
+    <t>breakdown (disruption)</t>
+  </si>
+  <si>
+    <t>Leukocyte-derived microvesicles</t>
+  </si>
+  <si>
+    <t>Endothelial microvesicles</t>
+  </si>
+  <si>
+    <t>direction</t>
+  </si>
+  <si>
+    <t>switch</t>
+  </si>
+  <si>
+    <t>INSERT</t>
   </si>
 </sst>
 </file>
@@ -1457,10 +1490,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1836,20 +1867,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D181B-FC1A-461E-92A1-3F55E3525786}">
-  <dimension ref="A1:E309"/>
+  <dimension ref="A1:F309"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="67.9296875" customWidth="1"/>
-    <col min="2" max="2" width="24.73046875" customWidth="1"/>
-    <col min="3" max="3" width="15.265625" customWidth="1"/>
+    <col min="2" max="2" width="28.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.73046875" customWidth="1"/>
+    <col min="4" max="4" width="21.53125" customWidth="1"/>
+    <col min="5" max="5" width="14.19921875" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1860,10 +1894,16 @@
         <v>310</v>
       </c>
       <c r="D1" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+        <v>315</v>
+      </c>
+      <c r="E1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1871,7 +1911,7 @@
         <v>73211009</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1879,7 +1919,7 @@
         <v>71395006</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1887,7 +1927,7 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1895,7 +1935,7 @@
         <v>59621000</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1903,7 +1943,7 @@
         <v>60621009</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1911,7 +1951,7 @@
         <v>49436004</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1919,7 +1959,7 @@
         <v>365981007</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1927,7 +1967,7 @@
         <v>55822004</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1935,7 +1975,7 @@
         <v>709044004</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1946,7 +1986,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1957,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1965,23 +2005,29 @@
         <v>246116008</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>276239002</v>
+      </c>
+      <c r="D14" t="s">
+        <v>318</v>
+      </c>
+      <c r="E14">
+        <v>103334006</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B15">
+        <v>246300000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1992,18 +2038,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>312</v>
       </c>
-      <c r="D17" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -2011,23 +2054,35 @@
         <v>49436004</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B19">
+        <v>439401001</v>
+      </c>
+      <c r="D19" t="s">
+        <v>318</v>
+      </c>
+      <c r="E19">
+        <v>103334006</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B20">
+        <v>716799009</v>
+      </c>
+      <c r="D20" t="s">
+        <v>319</v>
+      </c>
+      <c r="E20">
+        <v>36692007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -2035,10 +2090,13 @@
         <v>51308000</v>
       </c>
       <c r="D21" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+        <v>320</v>
+      </c>
+      <c r="E21">
+        <v>249032005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2046,10 +2104,13 @@
         <v>43810009</v>
       </c>
       <c r="D22" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+        <v>320</v>
+      </c>
+      <c r="E22">
+        <v>249032005</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -2057,7 +2118,7 @@
         <v>28960008</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -2065,7 +2126,7 @@
         <v>365981007</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -2073,7 +2134,7 @@
         <v>71395006</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -2081,7 +2142,7 @@
         <v>73211009</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -2089,7 +2150,7 @@
         <v>370992007</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -2097,7 +2158,7 @@
         <v>116661000</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -2105,7 +2166,7 @@
         <v>31996006</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -2113,7 +2174,7 @@
         <v>204317008</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -2121,7 +2182,7 @@
         <v>59621000</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -2132,7 +2193,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -2140,7 +2201,7 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -2148,7 +2209,7 @@
         <v>73211009</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -2156,7 +2217,7 @@
         <v>55822004</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -2164,7 +2225,7 @@
         <v>429775004</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2172,7 +2233,7 @@
         <v>226097005</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2180,7 +2241,7 @@
         <v>49436004</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -2188,7 +2249,7 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -2199,7 +2260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -2210,7 +2271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -2218,7 +2279,7 @@
         <v>59621000</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -2226,7 +2287,7 @@
         <v>51308000</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -2234,7 +2295,7 @@
         <v>246116008</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -2242,15 +2303,21 @@
         <v>60621009</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B46">
+        <v>27168002</v>
+      </c>
+      <c r="D46" t="s">
+        <v>321</v>
+      </c>
+      <c r="E46" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -2261,15 +2328,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.45">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -2277,15 +2344,15 @@
         <v>31996006</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -2293,7 +2360,7 @@
         <v>90708001</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -2301,7 +2368,7 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2309,7 +2376,7 @@
         <v>256235009</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2317,7 +2384,7 @@
         <v>370992007</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2325,10 +2392,13 @@
         <v>721961000000100</v>
       </c>
       <c r="D55" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.45">
+        <v>313</v>
+      </c>
+      <c r="E55">
+        <v>62482003</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2339,7 +2409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2347,7 +2417,7 @@
         <v>102680009</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2355,7 +2425,7 @@
         <v>56265001</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2363,7 +2433,7 @@
         <v>55235003</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2371,7 +2441,7 @@
         <v>226097005</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2379,7 +2449,7 @@
         <v>27550009</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2387,7 +2457,7 @@
         <v>35489007</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2395,7 +2465,7 @@
         <v>405056001</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2403,7 +2473,7 @@
         <v>160580001</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2411,7 +2481,7 @@
         <v>257552002</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2419,7 +2489,7 @@
         <v>386806002</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2427,7 +2497,7 @@
         <v>56675007</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2435,7 +2505,7 @@
         <v>260678004</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2443,7 +2513,7 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2451,7 +2521,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2459,10 +2529,13 @@
         <v>439127006</v>
       </c>
       <c r="D71" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.45">
+        <v>314</v>
+      </c>
+      <c r="E71">
+        <v>80891009</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2470,7 +2543,7 @@
         <v>48447003</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2478,7 +2551,7 @@
         <v>35489007</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2486,7 +2559,7 @@
         <v>122459003</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2494,7 +2567,7 @@
         <v>40739000</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2502,7 +2575,7 @@
         <v>104577001</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2510,7 +2583,7 @@
         <v>256235009</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2521,7 +2594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2532,7 +2605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2674,7 +2747,7 @@
         <v>22298006</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -2685,7 +2758,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -2693,7 +2766,7 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -2701,7 +2774,7 @@
         <v>260678004</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -2712,7 +2785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -2720,7 +2793,7 @@
         <v>73211009</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -2728,7 +2801,7 @@
         <v>459056003</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -2736,7 +2809,7 @@
         <v>160580001</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -2744,7 +2817,7 @@
         <v>73595000</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -2752,7 +2825,7 @@
         <v>315053001</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -2760,7 +2833,7 @@
         <v>116661000</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -2768,7 +2841,7 @@
         <v>308116003</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -2776,7 +2849,7 @@
         <v>233604007</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -2784,7 +2857,7 @@
         <v>429723008</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -2792,7 +2865,7 @@
         <v>40492006</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -2800,12 +2873,15 @@
         <v>38013005</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A112" t="s">
         <v>111</v>
       </c>
       <c r="B112">
-        <v>248152002</v>
+        <v>248153007</v>
+      </c>
+      <c r="F112" t="s">
+        <v>327</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -2820,7 +2896,7 @@
       <c r="A114" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114">
         <v>386725007</v>
       </c>
     </row>
@@ -2828,7 +2904,7 @@
       <c r="A115" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115">
         <v>2776000</v>
       </c>
     </row>
@@ -3064,7 +3140,7 @@
         <v>361071000000102</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A145" t="s">
         <v>144</v>
       </c>
@@ -3072,7 +3148,7 @@
         <v>315053001</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A146" t="s">
         <v>145</v>
       </c>
@@ -3080,7 +3156,7 @@
         <v>450741005</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A147" t="s">
         <v>146</v>
       </c>
@@ -3088,7 +3164,7 @@
         <v>724787004</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A148" t="s">
         <v>147</v>
       </c>
@@ -3096,7 +3172,7 @@
         <v>60621009</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A149" t="s">
         <v>148</v>
       </c>
@@ -3104,15 +3180,18 @@
         <v>73430006</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A150" t="s">
         <v>149</v>
       </c>
       <c r="B150">
-        <v>248152002</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.45">
+        <v>248153007</v>
+      </c>
+      <c r="F150" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A151" t="s">
         <v>150</v>
       </c>
@@ -3120,7 +3199,7 @@
         <v>4473006</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A152" t="s">
         <v>151</v>
       </c>
@@ -3128,7 +3207,7 @@
         <v>48194001</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A153" t="s">
         <v>152</v>
       </c>
@@ -3136,7 +3215,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A154" t="s">
         <v>153</v>
       </c>
@@ -3144,7 +3223,7 @@
         <v>237602007</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A155" t="s">
         <v>154</v>
       </c>
@@ -3152,15 +3231,21 @@
         <v>257552002</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A156" t="s">
         <v>155</v>
       </c>
-      <c r="B156" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B156">
+        <v>20245001</v>
+      </c>
+      <c r="D156" t="s">
+        <v>323</v>
+      </c>
+      <c r="E156">
+        <v>76555007</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A157" t="s">
         <v>156</v>
       </c>
@@ -3168,7 +3253,7 @@
         <v>89743005</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A158" t="s">
         <v>157</v>
       </c>
@@ -3176,7 +3261,7 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A159" t="s">
         <v>158</v>
       </c>
@@ -3184,7 +3269,7 @@
         <v>105981003</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A160" t="s">
         <v>159</v>
       </c>
@@ -3192,7 +3277,7 @@
         <v>415582006</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A161" t="s">
         <v>160</v>
       </c>
@@ -3200,7 +3285,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A162" t="s">
         <v>161</v>
       </c>
@@ -3208,7 +3293,7 @@
         <v>392031002</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A163" t="s">
         <v>162</v>
       </c>
@@ -3216,7 +3301,7 @@
         <v>1148582006</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A164" t="s">
         <v>163</v>
       </c>
@@ -3224,7 +3309,7 @@
         <v>6914000</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A165" t="s">
         <v>164</v>
       </c>
@@ -3232,7 +3317,7 @@
         <v>723857007</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A166" t="s">
         <v>165</v>
       </c>
@@ -3240,7 +3325,7 @@
         <v>398254007</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A167" t="s">
         <v>166</v>
       </c>
@@ -3248,7 +3333,7 @@
         <v>103579009</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A168" t="s">
         <v>167</v>
       </c>
@@ -3256,7 +3341,7 @@
         <v>47708004</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A169" t="s">
         <v>168</v>
       </c>
@@ -3264,7 +3349,7 @@
         <v>64779008</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A170" t="s">
         <v>169</v>
       </c>
@@ -3272,7 +3357,7 @@
         <v>363346000</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A171" t="s">
         <v>170</v>
       </c>
@@ -3280,7 +3365,7 @@
         <v>31996006</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A172" t="s">
         <v>171</v>
       </c>
@@ -3288,7 +3373,7 @@
         <v>367336001</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A173" t="s">
         <v>172</v>
       </c>
@@ -3296,15 +3381,18 @@
         <v>192759008</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A174" t="s">
         <v>173</v>
       </c>
       <c r="B174">
-        <v>248152002</v>
-      </c>
-    </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.45">
+        <v>248153007</v>
+      </c>
+      <c r="F174" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A175" t="s">
         <v>174</v>
       </c>
@@ -3312,7 +3400,7 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A176" t="s">
         <v>175</v>
       </c>
@@ -3448,7 +3536,7 @@
         <v>1325171000000100</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A193" t="s">
         <v>192</v>
       </c>
@@ -3456,7 +3544,7 @@
         <v>31653004</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A194" t="s">
         <v>193</v>
       </c>
@@ -3464,7 +3552,7 @@
         <v>31996006</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>194</v>
       </c>
@@ -3472,12 +3560,15 @@
         <v>69116000</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B196" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A197" t="s">
         <v>196</v>
       </c>
@@ -3485,17 +3576,23 @@
         <v>422504002</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A198" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B198" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A199" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B199">
+        <v>365782006</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A200" t="s">
         <v>199</v>
       </c>
@@ -3503,13 +3600,15 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A201" t="s">
         <v>200</v>
       </c>
-      <c r="E201" s="2"/>
-    </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B201">
+        <v>71395006</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A202" t="s">
         <v>201</v>
       </c>
@@ -3517,23 +3616,31 @@
         <v>13644009</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A203" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B203">
+        <v>414086009</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A204" t="s">
         <v>203</v>
       </c>
-      <c r="B204" s="2"/>
-    </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B204">
+        <v>439127006</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A205" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="B205">
+        <v>230698000</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A206" t="s">
         <v>205</v>
       </c>
@@ -3541,7 +3648,7 @@
         <v>49436004</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A207" t="s">
         <v>206</v>
       </c>
@@ -3549,72 +3656,117 @@
         <v>248153007</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A208" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B208">
+        <v>710864009</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A209" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B209">
+        <v>76612001</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A210" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B210" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A211" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B211">
+        <v>56265001</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A212" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B212">
+        <v>22298006</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A213" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B213">
+        <v>713142003</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A214" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B214">
+        <v>763325000</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A215" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B215">
+        <v>256235009</v>
+      </c>
+      <c r="F215" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A216" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B216">
+        <v>73595000</v>
+      </c>
+      <c r="D216" t="s">
+        <v>322</v>
+      </c>
+      <c r="E216">
+        <v>278926001</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A217" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B217">
+        <v>68365008</v>
+      </c>
+      <c r="D217" t="s">
+        <v>316</v>
+      </c>
+      <c r="E217">
+        <v>35105006</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A218" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
         <v>220</v>
       </c>
@@ -3622,7 +3774,7 @@
         <v>315053001</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A222" t="s">
         <v>221</v>
       </c>
@@ -3630,12 +3782,12 @@
         <v>89362005</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A223" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>223</v>
       </c>
@@ -3741,7 +3893,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A241" t="s">
         <v>240</v>
       </c>
@@ -3752,80 +3904,83 @@
         <v>2</v>
       </c>
     </row>
-    <row r="242" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A242" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="243" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="244" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="245" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="246" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="247" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="248" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
         <v>247</v>
       </c>
       <c r="B248">
-        <v>248152002</v>
-      </c>
-    </row>
-    <row r="249" spans="1:3" x14ac:dyDescent="0.45">
+        <v>248153007</v>
+      </c>
+      <c r="F248" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="250" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="251" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="252" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="253" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="254" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="255" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="256" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -4124,5 +4279,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
WISEDAG-12 finished snomed mapping, ready for review
</commit_message>
<xml_diff>
--- a/terms_excel.xlsx
+++ b/terms_excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leo\Desktop\Master Project\wise-dag\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CE0B17-0C88-4DB3-898F-9D6F27885C59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97C7CB0-FB10-4AE2-BFE4-976920993547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="11475" xr2:uid="{1724EB86-F306-47F4-ABEC-FB51705565F8}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="341">
   <si>
     <t>terms</t>
   </si>
@@ -985,28 +985,64 @@
     <t>rate of (speed of delivery)</t>
   </si>
   <si>
-    <t>dysfunction</t>
-  </si>
-  <si>
     <t>psychogenic</t>
   </si>
   <si>
     <t>breakdown (disruption)</t>
   </si>
   <si>
-    <t>Leukocyte-derived microvesicles</t>
-  </si>
-  <si>
-    <t>Endothelial microvesicles</t>
-  </si>
-  <si>
     <t>direction</t>
   </si>
   <si>
     <t>switch</t>
   </si>
   <si>
-    <t>INSERT</t>
+    <t>Endothelial microvesicles?</t>
+  </si>
+  <si>
+    <t>Leukocyte-derived microvesicles?</t>
+  </si>
+  <si>
+    <t>dysfunction/disorder</t>
+  </si>
+  <si>
+    <t>Revascularization</t>
+  </si>
+  <si>
+    <t>systemic</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t>localization</t>
+  </si>
+  <si>
+    <t>infiltration</t>
+  </si>
+  <si>
+    <t>brain</t>
+  </si>
+  <si>
+    <t>proliferation</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>neurologic</t>
+  </si>
+  <si>
+    <t>cerebral</t>
+  </si>
+  <si>
+    <t>peripheral</t>
+  </si>
+  <si>
+    <t>hemispheric</t>
+  </si>
+  <si>
+    <t>survival</t>
   </si>
 </sst>
 </file>
@@ -1869,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{906D181B-FC1A-461E-92A1-3F55E3525786}">
   <dimension ref="A1:F309"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47"/>
+    <sheetView tabSelected="1" topLeftCell="A293" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
+      <selection activeCell="C309" sqref="C309"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1900,7 +1936,7 @@
         <v>317</v>
       </c>
       <c r="F1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.45">
@@ -2311,10 +2347,10 @@
         <v>27168002</v>
       </c>
       <c r="D46" t="s">
-        <v>321</v>
-      </c>
-      <c r="E46" t="s">
-        <v>328</v>
+        <v>327</v>
+      </c>
+      <c r="E46">
+        <v>64572001</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.45">
@@ -2349,7 +2385,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.45">
@@ -2473,7 +2509,7 @@
         <v>160580001</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2481,15 +2517,18 @@
         <v>257552002</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>65</v>
       </c>
       <c r="B66">
-        <v>386806002</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+        <v>373930000</v>
+      </c>
+      <c r="F66" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2497,7 +2536,7 @@
         <v>56675007</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2505,7 +2544,7 @@
         <v>260678004</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2513,7 +2552,7 @@
         <v>38716007</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2521,7 +2560,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2535,7 +2574,7 @@
         <v>80891009</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2543,15 +2582,18 @@
         <v>48447003</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>72</v>
       </c>
       <c r="B73">
         <v>35489007</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="C73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2559,7 +2601,7 @@
         <v>122459003</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2567,7 +2609,7 @@
         <v>40739000</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2575,7 +2617,7 @@
         <v>104577001</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2583,7 +2625,7 @@
         <v>256235009</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2594,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2605,7 +2647,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2881,7 +2923,7 @@
         <v>248153007</v>
       </c>
       <c r="F112" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.45">
@@ -3129,7 +3171,7 @@
         <v>142</v>
       </c>
       <c r="B143">
-        <v>698456001</v>
+        <v>372720008</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.45">
@@ -3137,7 +3179,7 @@
         <v>143</v>
       </c>
       <c r="B144">
-        <v>361071000000102</v>
+        <v>840595002</v>
       </c>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.45">
@@ -3188,7 +3230,7 @@
         <v>248153007</v>
       </c>
       <c r="F150" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.45">
@@ -3239,7 +3281,7 @@
         <v>20245001</v>
       </c>
       <c r="D156" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E156">
         <v>76555007</v>
@@ -3389,7 +3431,7 @@
         <v>248153007</v>
       </c>
       <c r="F174" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.45">
@@ -3720,7 +3762,7 @@
         <v>256235009</v>
       </c>
       <c r="F215" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.45">
@@ -3731,7 +3773,7 @@
         <v>73595000</v>
       </c>
       <c r="D216" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E216">
         <v>278926001</v>
@@ -3755,16 +3797,25 @@
       <c r="A218" t="s">
         <v>217</v>
       </c>
+      <c r="B218">
+        <v>78275009</v>
+      </c>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A219" t="s">
         <v>218</v>
       </c>
+      <c r="B219">
+        <v>714628002</v>
+      </c>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A220" t="s">
         <v>219</v>
       </c>
+      <c r="B220">
+        <v>308116003</v>
+      </c>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A221" t="s">
@@ -3786,58 +3837,97 @@
       <c r="A223" t="s">
         <v>222</v>
       </c>
+      <c r="B223">
+        <v>437421000124105</v>
+      </c>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A224" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="225" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B224">
+        <v>226234005</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A225" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="226" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B225">
+        <v>418389000</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A226" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="227" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B226">
+        <v>372568004</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A227" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="228" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B227">
+        <v>703673007</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A228" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="229" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B228">
+        <v>416171004</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A229" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="230" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B229">
+        <v>47545007</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A230" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="231" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B230">
+        <v>440012000</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A231" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="232" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B231">
+        <v>69105007</v>
+      </c>
+      <c r="D231" t="s">
+        <v>328</v>
+      </c>
+      <c r="E231">
+        <v>297183000</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A232" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="233" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B232">
+        <v>840595002</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A233" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="234" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B233">
+        <v>260678004</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A234" t="s">
         <v>233</v>
       </c>
@@ -3845,7 +3935,7 @@
         <v>428202005</v>
       </c>
     </row>
-    <row r="235" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A235" t="s">
         <v>234</v>
       </c>
@@ -3853,7 +3943,7 @@
         <v>429775004</v>
       </c>
     </row>
-    <row r="236" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A236" t="s">
         <v>235</v>
       </c>
@@ -3861,7 +3951,7 @@
         <v>1161000175101</v>
       </c>
     </row>
-    <row r="237" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A237" t="s">
         <v>236</v>
       </c>
@@ -3872,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="238" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A238" t="s">
         <v>237</v>
       </c>
@@ -3883,14 +3973,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="239" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A239" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="240" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B239">
+        <v>257552002</v>
+      </c>
+      <c r="D239" t="s">
+        <v>329</v>
+      </c>
+      <c r="E239">
+        <v>31099001</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A240" t="s">
         <v>239</v>
+      </c>
+      <c r="B240">
+        <v>55641003</v>
+      </c>
+      <c r="D240" t="s">
+        <v>330</v>
+      </c>
+      <c r="E240">
+        <v>255509001</v>
       </c>
     </row>
     <row r="241" spans="1:6" x14ac:dyDescent="0.45">
@@ -3908,31 +4016,58 @@
       <c r="A242" t="s">
         <v>241</v>
       </c>
+      <c r="B242">
+        <v>203041005</v>
+      </c>
+      <c r="C242">
+        <v>2</v>
+      </c>
     </row>
     <row r="243" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A243" t="s">
         <v>242</v>
       </c>
+      <c r="B243">
+        <v>386806002</v>
+      </c>
     </row>
     <row r="244" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A244" t="s">
         <v>243</v>
       </c>
+      <c r="B244">
+        <v>55641003</v>
+      </c>
+      <c r="D244" t="s">
+        <v>331</v>
+      </c>
+      <c r="E244">
+        <v>257880008</v>
+      </c>
     </row>
     <row r="245" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A245" t="s">
         <v>244</v>
       </c>
+      <c r="B245">
+        <v>38013005</v>
+      </c>
     </row>
     <row r="246" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A246" t="s">
         <v>245</v>
       </c>
+      <c r="B246">
+        <v>221360009</v>
+      </c>
     </row>
     <row r="247" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A247" t="s">
         <v>246</v>
       </c>
+      <c r="B247">
+        <v>22253000</v>
+      </c>
     </row>
     <row r="248" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A248" t="s">
@@ -3942,80 +4077,128 @@
         <v>248153007</v>
       </c>
       <c r="F248" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="249" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A249" t="s">
         <v>248</v>
       </c>
+      <c r="B249">
+        <v>161045001</v>
+      </c>
     </row>
     <row r="250" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A250" t="s">
         <v>249</v>
       </c>
+      <c r="B250">
+        <v>2492009</v>
+      </c>
     </row>
     <row r="251" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A251" t="s">
         <v>250</v>
       </c>
+      <c r="B251">
+        <v>238108007</v>
+      </c>
     </row>
     <row r="252" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A252" t="s">
         <v>251</v>
       </c>
+      <c r="B252">
+        <v>87486003</v>
+      </c>
     </row>
     <row r="253" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A253" t="s">
         <v>252</v>
       </c>
+      <c r="B253">
+        <v>203041005</v>
+      </c>
+      <c r="C253">
+        <v>1</v>
+      </c>
     </row>
     <row r="254" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A254" t="s">
         <v>253</v>
       </c>
+      <c r="B254">
+        <v>35489007</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
     </row>
     <row r="255" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A255" t="s">
         <v>254</v>
       </c>
+      <c r="B255">
+        <v>41000005</v>
+      </c>
     </row>
     <row r="256" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A256" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B256">
+        <v>372720008</v>
+      </c>
+    </row>
+    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A257" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B257">
+        <v>5154007</v>
+      </c>
+    </row>
+    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A258" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B258">
+        <v>75516001</v>
+      </c>
+    </row>
+    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A259" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B259">
+        <v>91251008</v>
+      </c>
+    </row>
+    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A260" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B260">
+        <v>106328005</v>
+      </c>
+    </row>
+    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A261" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B261">
+        <v>315234002</v>
+      </c>
+    </row>
+    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A262" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B262">
+        <v>315233008</v>
+      </c>
+    </row>
+    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A263" t="s">
         <v>262</v>
       </c>
@@ -4023,77 +4206,173 @@
         <v>256235009</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A264" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B264">
+        <v>225351009</v>
+      </c>
+    </row>
+    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A265" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B265">
+        <v>278414003</v>
+      </c>
+    </row>
+    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A266" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B266">
+        <v>11894001</v>
+      </c>
+    </row>
+    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A267" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B267">
+        <v>302259009</v>
+      </c>
+    </row>
+    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A268" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B268">
+        <v>71395006</v>
+      </c>
+    </row>
+    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A269" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B269">
+        <v>112130006</v>
+      </c>
+      <c r="D269" t="s">
+        <v>332</v>
+      </c>
+      <c r="E269">
+        <v>47351003</v>
+      </c>
+    </row>
+    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A270" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B270">
+        <v>30965005</v>
+      </c>
+      <c r="D270" t="s">
+        <v>329</v>
+      </c>
+      <c r="E270">
+        <v>31099001</v>
+      </c>
+    </row>
+    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A271" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="272" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B271">
+        <v>30965005</v>
+      </c>
+      <c r="C271">
+        <v>1</v>
+      </c>
+      <c r="D271" t="s">
+        <v>333</v>
+      </c>
+      <c r="E271">
+        <v>12738006</v>
+      </c>
+    </row>
+    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A272" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="273" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B272">
+        <v>246329003</v>
+      </c>
+    </row>
+    <row r="273" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A273" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="274" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B273">
+        <v>27168002</v>
+      </c>
+      <c r="D273" t="s">
+        <v>334</v>
+      </c>
+      <c r="E273">
+        <v>30217000</v>
+      </c>
+    </row>
+    <row r="274" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A274" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="275" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B274">
+        <v>20245001</v>
+      </c>
+      <c r="D274" t="s">
+        <v>322</v>
+      </c>
+      <c r="E274">
+        <v>76555007</v>
+      </c>
+    </row>
+    <row r="275" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A275" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="276" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B275">
+        <v>63483002</v>
+      </c>
+      <c r="D275" t="s">
+        <v>334</v>
+      </c>
+      <c r="E275">
+        <v>30217000</v>
+      </c>
+    </row>
+    <row r="276" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A276" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="277" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B276">
+        <v>30965005</v>
+      </c>
+      <c r="C276">
+        <v>2</v>
+      </c>
+      <c r="D276" t="s">
+        <v>333</v>
+      </c>
+      <c r="E276">
+        <v>12738006</v>
+      </c>
+    </row>
+    <row r="277" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A277" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="278" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B277">
+        <v>78399007</v>
+      </c>
+      <c r="D277" t="s">
+        <v>334</v>
+      </c>
+      <c r="E277">
+        <v>30217000</v>
+      </c>
+    </row>
+    <row r="278" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A278" t="s">
         <v>277</v>
       </c>
@@ -4104,12 +4383,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="279" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A279" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="280" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B279">
+        <v>80274001</v>
+      </c>
+    </row>
+    <row r="280" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A280" t="s">
         <v>279</v>
       </c>
@@ -4120,108 +4402,177 @@
         <v>2</v>
       </c>
     </row>
-    <row r="281" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A281" t="s">
         <v>280</v>
       </c>
+      <c r="B281">
+        <v>840352000</v>
+      </c>
       <c r="C281">
         <v>2</v>
       </c>
     </row>
-    <row r="282" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A282" t="s">
         <v>281</v>
       </c>
+      <c r="B282">
+        <v>273302005</v>
+      </c>
       <c r="C282">
         <v>2</v>
       </c>
     </row>
-    <row r="283" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A283" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="284" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B283">
+        <v>12894003</v>
+      </c>
+    </row>
+    <row r="284" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A284" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="285" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B284">
+        <v>827181004</v>
+      </c>
+      <c r="D284" t="s">
+        <v>335</v>
+      </c>
+      <c r="E284">
+        <v>2603003</v>
+      </c>
+    </row>
+    <row r="285" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A285" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="286" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B285">
+        <v>409651001</v>
+      </c>
+    </row>
+    <row r="286" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A286" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="287" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B286">
+        <v>409651001</v>
+      </c>
+    </row>
+    <row r="287" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A287" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="288" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B287">
+        <v>414798009</v>
+      </c>
+    </row>
+    <row r="288" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A288" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B288">
+        <v>386806002</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A289" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="290" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B289">
+        <v>373930000</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A290" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="291" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B290">
+        <v>365812005</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A291" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="292" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B291">
+        <v>103326000</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A292" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="293" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B292">
+        <v>419620001</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A293" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="294" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B293">
+        <v>12894003</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A294" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="295" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B294">
+        <v>405152002</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A295" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="296" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B295">
+        <v>363803005</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A296" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="297" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B296">
+        <v>68349007</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A297" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="298" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B297" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A298" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="299" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B298">
+        <v>1131000119105</v>
+      </c>
+      <c r="D298" t="s">
+        <v>336</v>
+      </c>
+      <c r="E298">
+        <v>1199008</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A299" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="300" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B299">
+        <v>419620001</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -4232,49 +4583,103 @@
         <v>2</v>
       </c>
     </row>
-    <row r="301" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A301" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="302" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B301">
+        <v>257552002</v>
+      </c>
+      <c r="D301" t="s">
+        <v>337</v>
+      </c>
+      <c r="E301">
+        <v>12738006</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A302" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="303" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B302">
+        <v>106182000</v>
+      </c>
+      <c r="D302" t="s">
+        <v>338</v>
+      </c>
+      <c r="E302">
+        <v>14414005</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A303" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="304" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B303">
+        <v>419620001</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A304" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="305" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B304">
+        <v>405152002</v>
+      </c>
+      <c r="F304" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="305" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A305" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="306" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B305">
+        <v>268388007</v>
+      </c>
+    </row>
+    <row r="306" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A306" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="307" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B306">
+        <v>373930000</v>
+      </c>
+    </row>
+    <row r="307" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A307" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="308" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B307">
+        <v>90096001</v>
+      </c>
+    </row>
+    <row r="308" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A308" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="309" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="B308">
+        <v>13331008</v>
+      </c>
+      <c r="D308" t="s">
+        <v>339</v>
+      </c>
+      <c r="E308">
+        <v>21006006</v>
+      </c>
+    </row>
+    <row r="309" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A309" t="s">
         <v>308</v>
+      </c>
+      <c r="B309">
+        <v>47220008</v>
+      </c>
+      <c r="D309" t="s">
+        <v>340</v>
+      </c>
+      <c r="E309">
+        <v>724201000000108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>